<commit_message>
fixed overall wavsep results
</commit_message>
<xml_diff>
--- a/overall/overall-wavsep-results.xlsx
+++ b/overall/overall-wavsep-results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ranakhalil/Desktop/git/Thesis/results/overall/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ranakhalil/Desktop/git/Thesis-Test-Results/overall/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC81708B-CA1D-F247-9BC3-A7917CE97326}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAF9F31C-9DB9-A549-A38D-0A1EDFDAF0F0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="460" windowWidth="26640" windowHeight="15560" xr2:uid="{C657D2E9-8B8B-0F4B-8398-41FE36C22595}"/>
+    <workbookView xWindow="960" yWindow="460" windowWidth="26740" windowHeight="15940" xr2:uid="{C657D2E9-8B8B-0F4B-8398-41FE36C22595}"/>
   </bookViews>
   <sheets>
     <sheet name="TP" sheetId="1" r:id="rId1"/>
@@ -4542,7 +4542,7 @@
                   <c:v>0.2442622951</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.71311475410000003</c:v>
+                  <c:v>0.73770491800000004</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.7926229508</c:v>
@@ -4922,7 +4922,7 @@
                   <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.78260869570000002</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.86956521740000003</c:v>
@@ -6330,8 +6330,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71CABF22-ACF4-2E4A-9189-0F0FC55DE748}">
   <dimension ref="A1:C130"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A115" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C119" sqref="C119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -6410,7 +6410,7 @@
         <v>0.78260869570000002</v>
       </c>
       <c r="C7" s="5">
-        <v>0.78260869570000002</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -6998,7 +6998,7 @@
         <v>0.71311475410000003</v>
       </c>
       <c r="C129" s="5">
-        <v>0.71311475410000003</v>
+        <v>0.73770491800000004</v>
       </c>
     </row>
     <row r="130" spans="1:3">
@@ -7033,7 +7033,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FEC5E3E-73DE-EF4B-94F1-869472ED52B1}">
   <dimension ref="A2:C78"/>
   <sheetViews>
-    <sheetView topLeftCell="A60" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="A50" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="C82" sqref="C82"/>
     </sheetView>
   </sheetViews>

</xml_diff>